<commit_message>
more fungal ncbi genomes dno
</commit_message>
<xml_diff>
--- a/analyses/fungi-database-ncbi/fungal-db-summary.xlsx
+++ b/analyses/fungi-database-ncbi/fungal-db-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/fungi-database-ncbi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3260FAB7-CF9A-B648-A05A-7C3B8AA5BB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DC91B0-0300-C24C-87CF-93ED53894ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="3640" windowWidth="24640" windowHeight="13660" xr2:uid="{596C7BC3-5CCB-A047-8214-1D3C39C60451}"/>
+    <workbookView xWindow="4080" yWindow="2400" windowWidth="24640" windowHeight="13660" xr2:uid="{596C7BC3-5CCB-A047-8214-1D3C39C60451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="204">
   <si>
     <t xml:space="preserve">De novo LCA </t>
   </si>
@@ -65,28 +65,596 @@
     <t>multiisolate reference genome</t>
   </si>
   <si>
-    <t>YP_009254360.1</t>
-  </si>
-  <si>
     <t>Trichoderma gamsii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polytolypa hystricis </t>
+  </si>
+  <si>
+    <t>wood-degrader</t>
+  </si>
+  <si>
+    <t>PRJNA234736</t>
+  </si>
+  <si>
+    <t>monoisolate</t>
+  </si>
+  <si>
+    <t>biocontrol crop</t>
+  </si>
+  <si>
+    <t>medical</t>
+  </si>
+  <si>
+    <t>PRJNA322466</t>
+  </si>
+  <si>
+    <t>brown rot fungi</t>
+  </si>
+  <si>
+    <t>PRJNA342693</t>
+  </si>
+  <si>
+    <t>Ogataea polymorpha</t>
+  </si>
+  <si>
+    <t>yeast biotech</t>
+  </si>
+  <si>
+    <t>Chaetomium thermophilum</t>
+  </si>
+  <si>
+    <t>Fibularhizoctonia</t>
+  </si>
+  <si>
+    <t>Rozella allomycis</t>
+  </si>
+  <si>
+    <t>Verruconis gallopava</t>
+  </si>
+  <si>
+    <t>Diplocarpon rosae</t>
+  </si>
+  <si>
+    <t>Gonapodya prolifera</t>
+  </si>
+  <si>
+    <t>Amphiamblys</t>
+  </si>
+  <si>
+    <t>Macrophomina phaseolina</t>
+  </si>
+  <si>
+    <t>Penicillium camemberti</t>
+  </si>
+  <si>
+    <t>Hanseniaspora opuntiae</t>
+  </si>
+  <si>
+    <t>Rhizoctonia solani</t>
+  </si>
+  <si>
+    <t>Kazachstania africana</t>
+  </si>
+  <si>
+    <t>Aspergillus wentii</t>
+  </si>
+  <si>
+    <t>Trichoderma parareesei</t>
+  </si>
+  <si>
+    <t>Ophiocordyceps australis</t>
+  </si>
+  <si>
+    <t>Leucosporidium creatinivorum</t>
+  </si>
+  <si>
+    <t>Verticillium</t>
+  </si>
+  <si>
+    <t>Phellinus noxius</t>
+  </si>
+  <si>
+    <t>Rhodotorula toruloides</t>
+  </si>
+  <si>
+    <t>Paraphaeosphaeria sporulosa</t>
+  </si>
+  <si>
+    <t>Sporothrix insectorum</t>
+  </si>
+  <si>
+    <t>Polytolypa hystricis</t>
+  </si>
+  <si>
+    <t>Hypocreales</t>
+  </si>
+  <si>
+    <t>Pezizomycotina</t>
+  </si>
+  <si>
+    <t>Gaeumannomyces tritici</t>
+  </si>
+  <si>
+    <t>Paracoccidioides</t>
+  </si>
+  <si>
+    <t>Pseudogymnoascus</t>
+  </si>
+  <si>
+    <t>Penicillium occitanis</t>
+  </si>
+  <si>
+    <t>Trametes pubescens</t>
+  </si>
+  <si>
+    <t>Sordariomycetes</t>
+  </si>
+  <si>
+    <t>[Candida] auris</t>
+  </si>
+  <si>
+    <t>Kazachstania saulgeensis</t>
+  </si>
+  <si>
+    <t>Neocallimastix californiae</t>
+  </si>
+  <si>
+    <t>Serendipita indica</t>
+  </si>
+  <si>
+    <t>Clonostachys rosea</t>
+  </si>
+  <si>
+    <t>Hydnomerulius pinastri</t>
+  </si>
+  <si>
+    <t>Fusarium</t>
+  </si>
+  <si>
+    <t>Zymoseptoria brevis</t>
+  </si>
+  <si>
+    <t>Phialocephala subalpina</t>
+  </si>
+  <si>
+    <t>Mycena chlorophos</t>
+  </si>
+  <si>
+    <t>Malassezia pachydermatis</t>
+  </si>
+  <si>
+    <t>Stagonospora</t>
+  </si>
+  <si>
+    <t>Ganoderma sinense</t>
+  </si>
+  <si>
+    <t>Lodderomyces elongisporus</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces cryophilus</t>
+  </si>
+  <si>
+    <t>Kwoniella</t>
+  </si>
+  <si>
+    <t>Fusarium langsethiae</t>
+  </si>
+  <si>
+    <t>Penicillium oxalicum</t>
+  </si>
+  <si>
+    <t>Laccaria amethystina</t>
+  </si>
+  <si>
+    <t>Aspergillus</t>
+  </si>
+  <si>
+    <t>Pisolithus tinctorius</t>
+  </si>
+  <si>
+    <t>Diaporthe helianthi</t>
+  </si>
+  <si>
+    <t>Thielavia terrestris</t>
+  </si>
+  <si>
+    <t>Naumovozyma castellii</t>
+  </si>
+  <si>
+    <t>Exophiala xenobiotica</t>
+  </si>
+  <si>
+    <t>Amanita thiersii</t>
+  </si>
+  <si>
+    <t>Penicillium solitum</t>
+  </si>
+  <si>
+    <t>Sclerotinia borealis</t>
+  </si>
+  <si>
+    <t>Pezoloma ericae</t>
+  </si>
+  <si>
+    <t>Wickerhamomyces ciferrii</t>
+  </si>
+  <si>
+    <t>[Candida] pseudohaemulonis</t>
+  </si>
+  <si>
+    <t>[Candida] intermedia</t>
+  </si>
+  <si>
+    <t>Saitoella complicata</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces japonicus</t>
+  </si>
+  <si>
+    <t>Nematocida parisii</t>
+  </si>
+  <si>
+    <t>Mortierella elongata</t>
+  </si>
+  <si>
+    <t>Sporothrix brasiliensis</t>
+  </si>
+  <si>
+    <t>Tilletiaria anomala</t>
+  </si>
+  <si>
+    <t>Coccidioides immitis</t>
+  </si>
+  <si>
+    <t>Lobosporangium transversale</t>
+  </si>
+  <si>
+    <t>Clohesyomyces aquaticus</t>
+  </si>
+  <si>
+    <t>Hypoxylon</t>
+  </si>
+  <si>
+    <t>Claviceps purpurea</t>
+  </si>
+  <si>
+    <t>Lachancea mirantina</t>
+  </si>
+  <si>
+    <t>Torrubiella hemipterigena</t>
+  </si>
+  <si>
+    <t>Laetiporus sulphureus</t>
+  </si>
+  <si>
+    <t>Aspergillus clavatus</t>
+  </si>
+  <si>
+    <t>Tremellales</t>
+  </si>
+  <si>
+    <t>Aspergillus nidulans</t>
+  </si>
+  <si>
+    <t>Aspergillus turcosus</t>
+  </si>
+  <si>
+    <t>[Candida] glabrata</t>
+  </si>
+  <si>
+    <t>Tetrapisispora blattae</t>
+  </si>
+  <si>
+    <t>Rachicladosporium antarcticum</t>
+  </si>
+  <si>
+    <t>Candida parapsilosis</t>
+  </si>
+  <si>
+    <t>Rhizoclosmatium globosum</t>
+  </si>
+  <si>
+    <t>Leucoagaricus sp. SymC.cos</t>
+  </si>
+  <si>
+    <t>Serpula lacrymans var. lacrymans</t>
+  </si>
+  <si>
+    <t>Calocera viscosa</t>
+  </si>
+  <si>
+    <t>Neolentinus lepideus</t>
+  </si>
+  <si>
+    <t>Paracoccidioides lutzii</t>
+  </si>
+  <si>
+    <t>Dothistroma septosporum</t>
+  </si>
+  <si>
+    <t>Bipolaris</t>
+  </si>
+  <si>
+    <t>Histoplasma capsulatum</t>
+  </si>
+  <si>
+    <t>Colletotrichum higginsianum</t>
+  </si>
+  <si>
+    <t>Neocallimastigaceae</t>
+  </si>
+  <si>
+    <t>Ophiocordyceps camponoti-rufipedis</t>
+  </si>
+  <si>
+    <t>Pestalotiopsis fici</t>
+  </si>
+  <si>
+    <t>Sporothrix</t>
+  </si>
+  <si>
+    <t>Blastomyces</t>
+  </si>
+  <si>
+    <t>Metarhizium robertsii</t>
+  </si>
+  <si>
+    <t>Trichophyton</t>
+  </si>
+  <si>
+    <t>Leptosphaeria maculans</t>
+  </si>
+  <si>
+    <t>Millerozyma farinosa</t>
+  </si>
+  <si>
+    <t>Hypocreomycetidae</t>
+  </si>
+  <si>
+    <t>Baudoinia panamericana</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces pombe</t>
+  </si>
+  <si>
+    <t>Mixia osmundae</t>
+  </si>
+  <si>
+    <t>Candida</t>
+  </si>
+  <si>
+    <t>Naumovozyma dairenensis</t>
+  </si>
+  <si>
+    <t>Ophiocordyceps unilateralis</t>
+  </si>
+  <si>
+    <t>Tuber aestivum</t>
+  </si>
+  <si>
+    <t>Penicillium digitatum</t>
+  </si>
+  <si>
+    <t>Ophiostoma piceae</t>
+  </si>
+  <si>
+    <t>Tilletia indica</t>
+  </si>
+  <si>
+    <t>Laccaria</t>
+  </si>
+  <si>
+    <t>Acremonium chrysogenum</t>
+  </si>
+  <si>
+    <t>Fistulina hepatica</t>
+  </si>
+  <si>
+    <t>Colletotrichum</t>
+  </si>
+  <si>
+    <t>Rhizophagus irregularis</t>
+  </si>
+  <si>
+    <t>Rhodotorula</t>
+  </si>
+  <si>
+    <t>Emergomyces pasteurianus</t>
+  </si>
+  <si>
+    <t>Cladophialophora immunda</t>
+  </si>
+  <si>
+    <t>Metschnikowia bicuspidata var. bicuspidata</t>
+  </si>
+  <si>
+    <t>Hypocrella siamensis</t>
+  </si>
+  <si>
+    <t>Neolecta irregularis</t>
+  </si>
+  <si>
+    <t>Agaricomycetidae</t>
+  </si>
+  <si>
+    <t>Pyrenophora tritici-repentis</t>
+  </si>
+  <si>
+    <t>Exophiala oligosperma</t>
+  </si>
+  <si>
+    <t>Basidiobolus meristosporus</t>
+  </si>
+  <si>
+    <t>Peniophora sp. CONT</t>
+  </si>
+  <si>
+    <t>Cordyceps fumosorosea</t>
+  </si>
+  <si>
+    <t>Auricularia subglabra</t>
+  </si>
+  <si>
+    <t>Phanerochaete carnosa</t>
+  </si>
+  <si>
+    <t>Conidiobolus coronatus</t>
+  </si>
+  <si>
+    <t>Piloderma croceum</t>
+  </si>
+  <si>
+    <t>Pyronema omphalodes</t>
+  </si>
+  <si>
+    <t>Aureobasidium melanogenum</t>
+  </si>
+  <si>
+    <t>Coniosporium apollinis</t>
+  </si>
+  <si>
+    <t>Cladophialophora bantiana</t>
+  </si>
+  <si>
+    <t>Moelleriella libera</t>
+  </si>
+  <si>
+    <t>Calocera</t>
+  </si>
+  <si>
+    <t>Talaromyces stipitatus</t>
+  </si>
+  <si>
+    <t>Moniliophthora perniciosa</t>
+  </si>
+  <si>
+    <t>Rosellinia necatrix</t>
+  </si>
+  <si>
+    <t>Beauveria bassiana</t>
+  </si>
+  <si>
+    <t>Acidomyces richmondensis</t>
+  </si>
+  <si>
+    <t>Colletotrichum gloeosporioides</t>
+  </si>
+  <si>
+    <t>PRJNA225505</t>
+  </si>
+  <si>
+    <t>thermophile</t>
+  </si>
+  <si>
+    <t>PRJNA459569</t>
+  </si>
+  <si>
+    <t>bascidio</t>
+  </si>
+  <si>
+    <t>PRJNA421621</t>
+  </si>
+  <si>
+    <t>single cell</t>
+  </si>
+  <si>
+    <t>PRJNA325802</t>
+  </si>
+  <si>
+    <t>black yeast</t>
+  </si>
+  <si>
+    <t>PRJNA358006</t>
+  </si>
+  <si>
+    <t>black spot disease</t>
+  </si>
+  <si>
+    <t>PRJNA207863</t>
+  </si>
+  <si>
+    <t>digest algal cell walls</t>
+  </si>
+  <si>
+    <t>PRJNA321520</t>
+  </si>
+  <si>
+    <t>polychaete intestinal</t>
+  </si>
+  <si>
+    <t>environmental assembly</t>
+  </si>
+  <si>
+    <t>PRJNA577531</t>
+  </si>
+  <si>
+    <t>charcoal rot</t>
+  </si>
+  <si>
+    <t>PRJEB4962</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>PRJEB33345</t>
+  </si>
+  <si>
+    <t>biocontrol yeast</t>
+  </si>
+  <si>
+    <t>plant pathogen, widespread</t>
+  </si>
+  <si>
+    <t>PRJNA524447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiisolate </t>
+  </si>
+  <si>
+    <t>PRJNA178246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yeast </t>
+  </si>
+  <si>
+    <t>PRJNA358290</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>filamentous</t>
+  </si>
+  <si>
+    <t>PRJNA287603</t>
+  </si>
+  <si>
+    <t>PRJNA388689</t>
+  </si>
+  <si>
+    <t>PRJNA330695</t>
+  </si>
+  <si>
+    <t>PRJNA29511</t>
+  </si>
+  <si>
+    <t>hyhae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pezizomycotina </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,16 +677,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2225DE-4609-D14C-8A79-6EAD808717AD}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,7 +1010,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +1024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -471,8 +1037,11 @@
       <c r="D2">
         <v>11755</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -485,13 +1054,16 @@
       <c r="D3">
         <v>9930</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -499,11 +1071,1113 @@
       <c r="D4">
         <v>33455</v>
       </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>9934</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>5173</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>7164</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>1644</v>
+      </c>
+      <c r="E8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9">
+        <v>13037</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>11357</v>
+      </c>
+      <c r="E10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>13761</v>
+      </c>
+      <c r="E11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>13831</v>
+      </c>
+      <c r="E12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13">
+        <v>3642</v>
+      </c>
+      <c r="E13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>14667</v>
+      </c>
+      <c r="E14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>14418</v>
+      </c>
+      <c r="E15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>4192</v>
+      </c>
+      <c r="E16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17">
+        <v>85474</v>
+      </c>
+      <c r="E17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>5375</v>
+      </c>
+      <c r="E18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>12488</v>
+      </c>
+      <c r="E19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>9062</v>
+      </c>
+      <c r="E20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21">
+        <v>35036</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>9854</v>
+      </c>
+      <c r="E22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>10237</v>
+      </c>
+      <c r="E23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/bioproject/PRJNA64553/" xr:uid="{17323DE0-9DC9-E645-93E2-5F7A4C7333A7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>